<commit_message>
Création du fichier final
</commit_message>
<xml_diff>
--- a/LIVRABLE-3/Tests/Cahier de  tests MADERA.xlsx
+++ b/LIVRABLE-3/Tests/Cahier de  tests MADERA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\PFR\snir-co\LIVRABLE-3\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain.CHRETIEN\Documents\CESI\snir-co\LIVRABLE-3\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8182EDC-E2CB-4315-AFF7-A1221DF1D0AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DC40B9-FF92-4EA7-AFCC-151D8CD313CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47910399-D391-4954-945B-BD67CDF436A7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{47910399-D391-4954-945B-BD67CDF436A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
   <si>
     <t>Tests</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Créer un premier client</t>
   </si>
   <si>
-    <t>Un fiche récapitulative du client</t>
-  </si>
-  <si>
     <t>Création d'un plan</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Validation d'un projet</t>
   </si>
   <si>
-    <t>Après validation d'un projet création d'un devis</t>
-  </si>
-  <si>
     <t>US011</t>
   </si>
   <si>
@@ -283,13 +277,28 @@
   </si>
   <si>
     <t>Affichage d'un devis</t>
+  </si>
+  <si>
+    <t>Création d'un devis</t>
+  </si>
+  <si>
+    <t>Une fiche récapitulative du client</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>Pas de système de connexion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -322,8 +331,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,8 +357,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -386,11 +419,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -425,9 +497,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,6 +520,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -829,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE383F96-A5C9-4F13-8CD0-AEB7B6D00F6E}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -842,7 +926,7 @@
     <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -862,7 +946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -872,147 +956,145 @@
       <c r="C2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="D2" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="E3" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="26" t="s">
+        <v>84</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E7" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="26" t="s">
+        <v>84</v>
+      </c>
       <c r="F9" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E8:E9 E2:E6">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E8">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"KO"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9 E2:E8" xr:uid="{77D2D638-4263-48F3-8D7B-20D05D944105}">
-      <formula1>"OK,KO"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1020,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DE5CCC-80B7-4691-86DC-8B07BBD13895}">
   <dimension ref="A1:G1048556"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -1060,286 +1142,286 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>41</v>
+      <c r="B2" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>42</v>
+      <c r="B3" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>43</v>
+      <c r="B4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>44</v>
+      <c r="B5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>57</v>
+      <c r="A6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>45</v>
+      <c r="A7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>59</v>
+      <c r="B8" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>46</v>
+      <c r="A9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>47</v>
+      <c r="B10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>48</v>
+      <c r="B11" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="22"/>
+      <c r="C12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="21"/>
       <c r="E12" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="3"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C18" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C20" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C21" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C22" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C23" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C25" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C26" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C27" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C28" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C30" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C31" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C32" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C33" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C35" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C36" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C37" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D38" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1048556" spans="5:5" x14ac:dyDescent="0.2">
@@ -1568,18 +1650,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1602,6 +1684,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB90EC2-7DD6-482C-B81B-1F8DFD33BDB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47D5E28C-48D7-40C6-BF74-7D8971B440F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="12d5800f-c30f-4710-a751-5787a46b2072"/>
@@ -1616,12 +1706,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB90EC2-7DD6-482C-B81B-1F8DFD33BDB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>